<commit_message>
have issues with two backtracks
</commit_message>
<xml_diff>
--- a/report/A1/A1_v2.xlsx
+++ b/report/A1/A1_v2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Natsumeqi/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Natsumeqi/Google Drive/Concordia/2021Winter/1-COMP442/Assignments/COMP442-compiler-design/report/A1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{908D4505-3689-1246-B358-D0B7E722909E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F368CF92-8E50-5F4C-A522-EC893BF58CB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="460" windowWidth="19200" windowHeight="20080" xr2:uid="{0E8C4262-73D0-6446-A8AB-A1C01AC8BDB4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="47">
   <si>
     <t>L</t>
   </si>
@@ -555,7 +555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
+      <selection pane="bottomLeft" activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,7 +925,76 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6">
+        <v>17</v>
+      </c>
+      <c r="G6" s="6">
+        <v>17</v>
+      </c>
+      <c r="H6" s="6">
+        <v>17</v>
+      </c>
+      <c r="I6" s="6">
+        <v>17</v>
+      </c>
+      <c r="J6" s="6">
+        <v>17</v>
+      </c>
+      <c r="K6" s="6">
+        <v>17</v>
+      </c>
+      <c r="L6" s="6">
+        <v>17</v>
+      </c>
+      <c r="M6" s="6">
+        <v>17</v>
+      </c>
+      <c r="N6" s="6">
+        <v>17</v>
+      </c>
+      <c r="O6" s="6">
+        <v>17</v>
+      </c>
+      <c r="P6" s="6">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>17</v>
+      </c>
+      <c r="R6" s="6">
+        <v>17</v>
+      </c>
+      <c r="S6" s="6">
+        <v>17</v>
+      </c>
+      <c r="T6" s="6">
+        <v>17</v>
+      </c>
+      <c r="U6" s="6">
+        <v>17</v>
+      </c>
+      <c r="V6" s="6">
+        <v>17</v>
+      </c>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+    </row>
     <row r="7" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>5</v>
@@ -1212,145 +1281,145 @@
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
-    <row r="11" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
+    <row r="11" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="6">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
+        <v>9</v>
+      </c>
+      <c r="E11" s="6">
+        <v>9</v>
+      </c>
+      <c r="F11" s="6">
+        <v>17</v>
+      </c>
+      <c r="G11" s="6">
+        <v>17</v>
+      </c>
+      <c r="H11" s="6">
+        <v>17</v>
+      </c>
+      <c r="I11" s="6">
+        <v>17</v>
+      </c>
+      <c r="J11" s="6">
+        <v>17</v>
+      </c>
+      <c r="K11" s="6">
+        <v>17</v>
+      </c>
+      <c r="L11" s="6">
+        <v>17</v>
+      </c>
+      <c r="M11" s="6">
+        <v>17</v>
+      </c>
+      <c r="N11" s="6">
+        <v>17</v>
+      </c>
+      <c r="O11" s="6">
+        <v>17</v>
+      </c>
+      <c r="P11" s="6">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>17</v>
+      </c>
+      <c r="R11" s="6">
+        <v>17</v>
+      </c>
+      <c r="S11" s="6">
+        <v>17</v>
+      </c>
+      <c r="T11" s="6">
+        <v>17</v>
+      </c>
+      <c r="U11" s="6">
+        <v>17</v>
+      </c>
+      <c r="V11" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="C11" s="5">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5">
-        <v>9</v>
-      </c>
-      <c r="E11" s="5">
-        <v>9</v>
-      </c>
-      <c r="F11" s="5">
-        <v>10</v>
-      </c>
-      <c r="G11" s="5">
-        <v>10</v>
-      </c>
-      <c r="H11" s="5">
-        <v>10</v>
-      </c>
-      <c r="I11" s="5">
-        <v>10</v>
-      </c>
-      <c r="J11" s="5">
-        <v>10</v>
-      </c>
-      <c r="K11" s="5">
-        <v>10</v>
-      </c>
-      <c r="L11" s="5">
-        <v>10</v>
-      </c>
-      <c r="M11" s="5">
-        <v>10</v>
-      </c>
-      <c r="N11" s="5">
-        <v>9</v>
-      </c>
-      <c r="O11" s="5">
-        <v>9</v>
-      </c>
-      <c r="P11" s="5">
-        <v>10</v>
-      </c>
-      <c r="Q11" s="5">
-        <v>9</v>
-      </c>
-      <c r="R11" s="5">
-        <v>10</v>
-      </c>
-      <c r="S11" s="5">
-        <v>10</v>
-      </c>
-      <c r="T11" s="5">
-        <v>10</v>
-      </c>
-      <c r="U11" s="5">
-        <v>0</v>
-      </c>
-      <c r="V11" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1</v>
-      </c>
-      <c r="G12" s="5">
-        <v>1</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1</v>
-      </c>
-      <c r="I12" s="5">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5">
-        <v>1</v>
-      </c>
-      <c r="K12" s="5">
-        <v>1</v>
-      </c>
-      <c r="L12" s="5">
-        <v>1</v>
-      </c>
-      <c r="M12" s="5">
-        <v>1</v>
-      </c>
-      <c r="N12" s="5">
-        <v>1</v>
-      </c>
-      <c r="O12" s="5">
-        <v>1</v>
-      </c>
-      <c r="P12" s="5">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="5">
-        <v>1</v>
-      </c>
-      <c r="R12" s="5">
-        <v>1</v>
-      </c>
-      <c r="S12" s="5">
-        <v>1</v>
-      </c>
-      <c r="T12" s="5">
-        <v>1</v>
-      </c>
-      <c r="U12" s="5">
-        <v>1</v>
-      </c>
-      <c r="V12" s="5">
-        <v>1</v>
-      </c>
-      <c r="W12" s="5" t="s">
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <v>1</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1</v>
+      </c>
+      <c r="M12" s="6">
+        <v>1</v>
+      </c>
+      <c r="N12" s="6">
+        <v>1</v>
+      </c>
+      <c r="O12" s="6">
+        <v>1</v>
+      </c>
+      <c r="P12" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="6">
+        <v>1</v>
+      </c>
+      <c r="R12" s="6">
+        <v>1</v>
+      </c>
+      <c r="S12" s="6">
+        <v>1</v>
+      </c>
+      <c r="T12" s="6">
+        <v>1</v>
+      </c>
+      <c r="U12" s="6">
+        <v>1</v>
+      </c>
+      <c r="V12" s="6">
+        <v>1</v>
+      </c>
+      <c r="W12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="X12" s="5" t="s">
+      <c r="X12" s="6" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1428,72 +1497,78 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+    <row r="14" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="5">
-        <v>12</v>
-      </c>
-      <c r="C14" s="5">
-        <v>12</v>
-      </c>
-      <c r="D14" s="5">
-        <v>5</v>
-      </c>
-      <c r="E14" s="5">
-        <v>5</v>
-      </c>
-      <c r="F14" s="5">
-        <v>5</v>
-      </c>
-      <c r="G14" s="5">
-        <v>5</v>
-      </c>
-      <c r="H14" s="5">
-        <v>5</v>
-      </c>
-      <c r="I14" s="5">
-        <v>5</v>
-      </c>
-      <c r="J14" s="5">
-        <v>5</v>
-      </c>
-      <c r="K14" s="5">
-        <v>5</v>
-      </c>
-      <c r="L14" s="5">
-        <v>5</v>
-      </c>
-      <c r="M14" s="5">
-        <v>5</v>
-      </c>
-      <c r="N14" s="5">
-        <v>5</v>
-      </c>
-      <c r="O14" s="5">
-        <v>5</v>
-      </c>
-      <c r="P14" s="5">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="5">
-        <v>5</v>
-      </c>
-      <c r="R14" s="5">
-        <v>5</v>
-      </c>
-      <c r="S14" s="5">
-        <v>5</v>
-      </c>
-      <c r="T14" s="5">
-        <v>5</v>
-      </c>
-      <c r="U14" s="5">
-        <v>0</v>
-      </c>
-      <c r="V14" s="5">
-        <v>5</v>
+      <c r="B14" s="6">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
+        <v>1</v>
+      </c>
+      <c r="K14" s="6">
+        <v>1</v>
+      </c>
+      <c r="L14" s="6">
+        <v>1</v>
+      </c>
+      <c r="M14" s="6">
+        <v>1</v>
+      </c>
+      <c r="N14" s="6">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6">
+        <v>1</v>
+      </c>
+      <c r="P14" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="6">
+        <v>1</v>
+      </c>
+      <c r="R14" s="6">
+        <v>1</v>
+      </c>
+      <c r="S14" s="6">
+        <v>1</v>
+      </c>
+      <c r="T14" s="6">
+        <v>1</v>
+      </c>
+      <c r="U14" s="6">
+        <v>1</v>
+      </c>
+      <c r="V14" s="6">
+        <v>1</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X14" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -1581,61 +1656,61 @@
         <v>7</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E16">
         <v>15</v>
       </c>
       <c r="F16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="K16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="M16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="P16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="R16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="S16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="T16">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="U16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V16">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.2">
@@ -1643,7 +1718,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C17">
         <v>18</v>
@@ -1700,78 +1775,78 @@
         <v>17</v>
       </c>
       <c r="U17">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="V17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+    <row r="18" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="6">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6">
+        <v>10</v>
+      </c>
+      <c r="D18" s="6">
         <v>16</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>15</v>
       </c>
-      <c r="F18">
-        <v>7</v>
-      </c>
-      <c r="G18">
-        <v>7</v>
-      </c>
-      <c r="H18">
-        <v>7</v>
-      </c>
-      <c r="I18">
-        <v>7</v>
-      </c>
-      <c r="J18">
-        <v>7</v>
-      </c>
-      <c r="K18">
-        <v>7</v>
-      </c>
-      <c r="L18">
-        <v>7</v>
-      </c>
-      <c r="M18">
-        <v>7</v>
-      </c>
-      <c r="N18">
-        <v>7</v>
-      </c>
-      <c r="O18">
-        <v>7</v>
-      </c>
-      <c r="P18">
-        <v>7</v>
-      </c>
-      <c r="Q18">
-        <v>7</v>
-      </c>
-      <c r="R18">
-        <v>7</v>
-      </c>
-      <c r="S18">
-        <v>7</v>
-      </c>
-      <c r="T18">
-        <v>7</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-      <c r="V18">
-        <v>7</v>
+      <c r="F18" s="6">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6">
+        <v>10</v>
+      </c>
+      <c r="H18" s="6">
+        <v>10</v>
+      </c>
+      <c r="I18" s="6">
+        <v>10</v>
+      </c>
+      <c r="J18" s="6">
+        <v>10</v>
+      </c>
+      <c r="K18" s="6">
+        <v>10</v>
+      </c>
+      <c r="L18" s="6">
+        <v>10</v>
+      </c>
+      <c r="M18" s="6">
+        <v>10</v>
+      </c>
+      <c r="N18" s="6">
+        <v>10</v>
+      </c>
+      <c r="O18" s="6">
+        <v>10</v>
+      </c>
+      <c r="P18" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>10</v>
+      </c>
+      <c r="R18" s="6">
+        <v>10</v>
+      </c>
+      <c r="S18" s="6">
+        <v>10</v>
+      </c>
+      <c r="T18" s="6">
+        <v>10</v>
+      </c>
+      <c r="U18" s="6">
+        <v>10</v>
+      </c>
+      <c r="V18" s="6">
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.2">
@@ -1853,40 +1928,40 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D20">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E20">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="K20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="M20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="N20">
         <v>19</v>
@@ -1895,25 +1970,25 @@
         <v>19</v>
       </c>
       <c r="P20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="Q20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="R20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="S20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="T20">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="U20">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="V20">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
@@ -1921,134 +1996,134 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E21">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="J21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="K21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="L21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="M21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="N21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="O21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="P21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="Q21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="R21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="S21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="T21">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="V21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>7</v>
-      </c>
-      <c r="D22">
+      <c r="B22" s="5">
+        <v>7</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7</v>
+      </c>
+      <c r="D22" s="5">
         <v>20</v>
       </c>
-      <c r="E22">
-        <v>7</v>
-      </c>
-      <c r="F22">
-        <v>7</v>
-      </c>
-      <c r="G22">
-        <v>7</v>
-      </c>
-      <c r="H22">
-        <v>7</v>
-      </c>
-      <c r="I22">
-        <v>7</v>
-      </c>
-      <c r="J22">
-        <v>7</v>
-      </c>
-      <c r="K22">
-        <v>7</v>
-      </c>
-      <c r="L22">
-        <v>7</v>
-      </c>
-      <c r="M22">
-        <v>7</v>
-      </c>
-      <c r="N22">
-        <v>7</v>
-      </c>
-      <c r="O22">
-        <v>7</v>
-      </c>
-      <c r="P22">
-        <v>7</v>
-      </c>
-      <c r="Q22">
-        <v>17</v>
-      </c>
-      <c r="R22">
-        <v>17</v>
-      </c>
-      <c r="S22">
-        <v>17</v>
-      </c>
-      <c r="T22">
-        <v>17</v>
-      </c>
-      <c r="U22">
+      <c r="E22" s="5">
+        <v>7</v>
+      </c>
+      <c r="F22" s="5">
+        <v>7</v>
+      </c>
+      <c r="G22" s="5">
+        <v>7</v>
+      </c>
+      <c r="H22" s="5">
+        <v>7</v>
+      </c>
+      <c r="I22" s="5">
+        <v>7</v>
+      </c>
+      <c r="J22" s="5">
+        <v>7</v>
+      </c>
+      <c r="K22" s="5">
+        <v>7</v>
+      </c>
+      <c r="L22" s="5">
+        <v>7</v>
+      </c>
+      <c r="M22" s="5">
+        <v>7</v>
+      </c>
+      <c r="N22" s="5">
+        <v>7</v>
+      </c>
+      <c r="O22" s="5">
+        <v>7</v>
+      </c>
+      <c r="P22" s="5">
+        <v>7</v>
+      </c>
+      <c r="Q22" s="5">
+        <v>17</v>
+      </c>
+      <c r="R22" s="5">
+        <v>17</v>
+      </c>
+      <c r="S22" s="5">
+        <v>17</v>
+      </c>
+      <c r="T22" s="5">
+        <v>17</v>
+      </c>
+      <c r="U22" s="5">
         <v>0</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="5">
         <v>17</v>
       </c>
     </row>
@@ -2120,71 +2195,71 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-      <c r="C24">
-        <v>7</v>
-      </c>
-      <c r="D24">
+      <c r="B24" s="5">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5">
         <v>22</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="5">
         <v>22</v>
       </c>
-      <c r="F24">
-        <v>17</v>
-      </c>
-      <c r="G24">
-        <v>17</v>
-      </c>
-      <c r="H24">
-        <v>17</v>
-      </c>
-      <c r="I24">
-        <v>17</v>
-      </c>
-      <c r="J24">
-        <v>17</v>
-      </c>
-      <c r="K24">
-        <v>17</v>
-      </c>
-      <c r="L24">
-        <v>17</v>
-      </c>
-      <c r="M24">
-        <v>17</v>
-      </c>
-      <c r="N24">
-        <v>17</v>
-      </c>
-      <c r="O24">
-        <v>17</v>
-      </c>
-      <c r="P24">
-        <v>17</v>
-      </c>
-      <c r="Q24">
-        <v>17</v>
-      </c>
-      <c r="R24">
-        <v>17</v>
-      </c>
-      <c r="S24">
-        <v>17</v>
-      </c>
-      <c r="T24">
-        <v>17</v>
-      </c>
-      <c r="U24">
+      <c r="F24" s="5">
+        <v>17</v>
+      </c>
+      <c r="G24" s="5">
+        <v>17</v>
+      </c>
+      <c r="H24" s="5">
+        <v>17</v>
+      </c>
+      <c r="I24" s="5">
+        <v>17</v>
+      </c>
+      <c r="J24" s="5">
+        <v>17</v>
+      </c>
+      <c r="K24" s="5">
+        <v>17</v>
+      </c>
+      <c r="L24" s="5">
+        <v>17</v>
+      </c>
+      <c r="M24" s="5">
+        <v>17</v>
+      </c>
+      <c r="N24" s="5">
+        <v>17</v>
+      </c>
+      <c r="O24" s="5">
+        <v>17</v>
+      </c>
+      <c r="P24" s="5">
+        <v>17</v>
+      </c>
+      <c r="Q24" s="5">
+        <v>17</v>
+      </c>
+      <c r="R24" s="5">
+        <v>17</v>
+      </c>
+      <c r="S24" s="5">
+        <v>17</v>
+      </c>
+      <c r="T24" s="5">
+        <v>17</v>
+      </c>
+      <c r="U24" s="5">
         <v>0</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="5">
         <v>17</v>
       </c>
     </row>

</xml_diff>